<commit_message>
adjust the directory structure and implement selenium grid dockerize and cross browser testing
</commit_message>
<xml_diff>
--- a/SeleniumProject/TestDataAccess/userdataTest.xlsx
+++ b/SeleniumProject/TestDataAccess/userdataTest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\repo\c-sharp-project\seleniumCs\seleniumCs\TestDataAccess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\repo\SeleniumCSharp\SeleniumProject\TestDataAccess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF89CDD-4F81-4A9C-AB89-B20F27101754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C935B7-FA71-45A7-9359-5CA28AF54FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{20182629-DC4E-49DF-8A70-9E1E03754C59}"/>
+    <workbookView xWindow="5760" yWindow="588" windowWidth="17280" windowHeight="8880" xr2:uid="{20182629-DC4E-49DF-8A70-9E1E03754C59}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTest" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <t>UnitTest1</t>
   </si>
   <si>
-    <t>Password1234</t>
+    <t>Password123</t>
   </si>
 </sst>
 </file>

</xml_diff>